<commit_message>
update code tao report luong tai report co so
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Đơn sale chính" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Lương" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Đơn sale phụ" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Lương" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,19 +415,365 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tiền tố</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mã dịch vụ</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ngày thực hiện</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Cơ sở</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Khách hàng</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Nguồn khách</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Tên dịch vụ</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Đơn giá gốc</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Sale phụ</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Upsale</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Đơn giá</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Đã thanh toán</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Tỉ lệ chiết khấu sale chính</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Chiết khấu sale chính</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>615</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>08-01-2024</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Nguyễn Thị Mỹ Duyên</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Khách cũ</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Tiêm Filler</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>2100000</v>
+      </c>
+      <c r="I2" t="n">
+        <v/>
+      </c>
+      <c r="J2" t="n">
+        <v/>
+      </c>
+      <c r="K2" t="n">
+        <v>2100000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2100000</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tổng</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>2100000</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2100000</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2100000</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>210000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tiền tố</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mã dịch vụ</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ngày thực hiện</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Cơ sở</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Khách hàng</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Nguồn khách</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Tên dịch vụ</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Đơn giá gốc</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Sale phụ</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Upsale</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Đơn giá</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Đã thanh toán</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Tỉ lệ chiết khấu sale phụ</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Chiết khấu sale phụ</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>614</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>08-01-2024</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Trần Nguyễn Yến Linh</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Khách cũ</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Cắt mí</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Đỗ Thị Huyền Trân</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="K2" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N2" t="n">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tổng</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="K3" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="L3" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>240000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -457,7 +804,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -467,7 +814,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="4">
@@ -477,7 +824,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>357142.8571428572</v>
       </c>
     </row>
     <row r="5">
@@ -487,7 +834,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="6">
@@ -497,7 +844,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>240000</v>
       </c>
     </row>
     <row r="7">
@@ -757,7 +1104,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>877142.8571428572</v>
       </c>
     </row>
     <row r="33">
@@ -783,11 +1130,11 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Tổng lương</t>
+          <t>Tổng lương tại HỆ THỐNG</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>877142.8571428572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix lỗi trong report cơ sở. Thêm cột ghi chú trong báo cáo về chi tiêu
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="Đơn sale chính" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Đơn sale phụ" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Lương" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Đơn thu nợ" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Lương" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -596,7 +597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -737,35 +738,151 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>629</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>08-05-2024</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Phạm Thị Trúc Lài</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>CTV</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Phun mày</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>500000</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Đỗ Thị Huyền Trân</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>500000</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N3" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>631</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>08-06-2024</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Võ Thị Thuỳ Trang</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>CTV</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Phun mày</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>500000</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Đỗ Thị Huyền Trân</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N4" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>6000000</v>
-      </c>
-      <c r="K3" t="n">
-        <v>6000000</v>
-      </c>
-      <c r="L3" t="n">
-        <v>6000000</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>240000</v>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>7500000</v>
+      </c>
+      <c r="K5" t="n">
+        <v>8500000</v>
+      </c>
+      <c r="L5" t="n">
+        <v>8500000</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>270000</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +896,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -790,6 +907,308 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Tiền tố</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mã đơn thu nợ</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Lượng thu</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Ngày thu</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Cơ sở</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Đơn nợ</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Tên dịch vụ</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Khách hàng</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Nguồn khách</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Sale chính</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Đơn giá gốc</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Sale phụ</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Upsale</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Đơn giá</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Đã thanh toán</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Bác sĩ 1</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Bác sĩ 2</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Tỉ lệ chiết khấu sale chính</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Chiết khấu sale chính</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Tỉ lệ chiết khấu sale phụ</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Chiết khấu sale phụ</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Tỉ lệ chiết khấu bác sĩ 1</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Chiết khấu bác sĩ 1</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>Tỉ lệ chiết khấu bác sĩ 2</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>Chiết khấu bác sĩ 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>181</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>08-09-2024</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>HD-LUXURY-538</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Nâng mũi</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Ngô Xuân Nhi</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Lâm Hoàng Phú</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Đỗ Thị Huyền Trân</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="N2" t="n">
+        <v>18000000</v>
+      </c>
+      <c r="O2" t="n">
+        <v>11000000</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Lâm Thị Mỹ Hằng</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v/>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="U2" t="n">
+        <v>40000</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tổng</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="N3" t="n">
+        <v>18000000</v>
+      </c>
+      <c r="O3" t="n">
+        <v>11000000</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>40000</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>Danh mục lương</t>
         </is>
       </c>
@@ -804,7 +1223,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="3">
@@ -814,7 +1233,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>70000</v>
+        <v>227500</v>
       </c>
     </row>
     <row r="4">
@@ -824,7 +1243,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>357142.8571428572</v>
+        <v>1160714.285714286</v>
       </c>
     </row>
     <row r="5">
@@ -844,7 +1263,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>240000</v>
+        <v>270000</v>
       </c>
     </row>
     <row r="7">
@@ -890,17 +1309,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ứng lương tại CẦN THƠ</t>
+          <t>Chiết khấu thu nợ tại CẦN THƠ</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Tổng công tại LONG XUYÊN</t>
+          <t>Ứng lương tại CẦN THƠ</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -910,7 +1329,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Lương công tác tại LONG XUYÊN</t>
+          <t>Tổng công tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -920,27 +1339,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Lương cơ bản tại LONG XUYÊN</t>
+          <t>Lương công tác tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Chiết khấu sale chính tại LONG XUYÊN</t>
+          <t>Lương cơ bản tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Chiết khấu sale phụ tại LONG XUYÊN</t>
+          <t>Chiết khấu sale chính tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -950,7 +1369,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Đơn 1 bác sĩ tại LONG XUYÊN</t>
+          <t>Chiết khấu sale phụ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -960,7 +1379,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Đơn 2 bác sĩ tại LONG XUYÊN</t>
+          <t>Đơn 1 bác sĩ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -970,7 +1389,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 1 tại LONG XUYÊN</t>
+          <t>Đơn 2 bác sĩ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -980,7 +1399,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 2 tại LONG XUYÊN</t>
+          <t>Công phụ phẫu 1 tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -990,7 +1409,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ứng lương tại LONG XUYÊN</t>
+          <t>Công phụ phẫu 2 tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1000,7 +1419,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Tổng công tại SÓC TRĂNG</t>
+          <t>Chiết khấu thu nợ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1010,7 +1429,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Lương công tác tại SÓC TRĂNG</t>
+          <t>Ứng lương tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1020,17 +1439,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Lương cơ bản tại SÓC TRĂNG</t>
+          <t>Tổng công tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Chiết khấu sale chính tại SÓC TRĂNG</t>
+          <t>Lương công tác tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1040,17 +1459,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Chiết khấu sale phụ tại SÓC TRĂNG</t>
+          <t>Lương cơ bản tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Đơn 1 bác sĩ tại SÓC TRĂNG</t>
+          <t>Chiết khấu sale chính tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1060,7 +1479,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Đơn 2 bác sĩ tại SÓC TRĂNG</t>
+          <t>Chiết khấu sale phụ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1070,7 +1489,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 1 tại SÓC TRĂNG</t>
+          <t>Đơn 1 bác sĩ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1080,7 +1499,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 2 tại SÓC TRĂNG</t>
+          <t>Đơn 2 bác sĩ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1090,7 +1509,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ứng lương tại SÓC TRĂNG</t>
+          <t>Công phụ phẫu 1 tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1100,17 +1519,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Tổng lương tại CẦN THƠ</t>
+          <t>Công phụ phẫu 2 tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>877142.8571428572</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Tổng lương tại LONG XUYÊN</t>
+          <t>Chiết khấu thu nợ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1120,7 +1539,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Tổng lương tại SÓC TRĂNG</t>
+          <t>Ứng lương tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1130,11 +1549,41 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>Tổng lương tại CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1908214.285714286</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Tổng lương tại LONG XUYÊN</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Tổng lương tại SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
           <t>Tổng lương tại HỆ THỐNG</t>
         </is>
       </c>
-      <c r="B35" t="n">
-        <v>877142.8571428572</v>
+      <c r="B38" t="n">
+        <v>1908214.285714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code thêm tạo report lương tổng hợp
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,35 +555,91 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>643</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>08-11-2024</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Trần Thị Nhi</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Cắt mí</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="I3" t="n">
+        <v/>
+      </c>
+      <c r="J3" t="n">
+        <v/>
+      </c>
+      <c r="K3" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="L3" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>2100000</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>2100000</v>
-      </c>
-      <c r="L3" t="n">
-        <v>2100000</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>210000</v>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>5100000</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>5100000</v>
+      </c>
+      <c r="L4" t="n">
+        <v>5100000</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>510000</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1279,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="3">
@@ -1233,7 +1289,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>227500</v>
+        <v>332500</v>
       </c>
     </row>
     <row r="4">
@@ -1243,7 +1299,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1160714.285714286</v>
+        <v>1696428.571428572</v>
       </c>
     </row>
     <row r="5">
@@ -1253,7 +1309,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>210000</v>
+        <v>510000</v>
       </c>
     </row>
     <row r="6">
@@ -1553,7 +1609,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1908214.285714286</v>
+        <v>2848928.571428572</v>
       </c>
     </row>
     <row r="36">
@@ -1583,7 +1639,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1908214.285714286</v>
+        <v>2848928.571428572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug trong file convertJsonToExcel
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -891,35 +891,147 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>675</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>08-23-2024</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Đoàn Minh Thư</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Tiêm Filler</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v/>
+      </c>
+      <c r="I9" t="n">
+        <v/>
+      </c>
+      <c r="J9" t="n">
+        <v/>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>676</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>08-23-2024</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Nguyễn Thị Ngọc Tâm</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Khách cũ</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Tiêm Filler</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>3700000</v>
+      </c>
+      <c r="I10" t="n">
+        <v/>
+      </c>
+      <c r="J10" t="n">
+        <v/>
+      </c>
+      <c r="K10" t="n">
+        <v>3700000</v>
+      </c>
+      <c r="L10" t="n">
+        <v>3700000</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N10" t="n">
+        <v>370000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>7</v>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
-        <v>24600000</v>
-      </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>24600000</v>
-      </c>
-      <c r="L9" t="n">
-        <v>24600000</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>2622000</v>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>28300000</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>28300000</v>
+      </c>
+      <c r="L11" t="n">
+        <v>29800000</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>2992000</v>
       </c>
     </row>
   </sheetData>
@@ -1290,7 +1402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1487,7 +1599,7 @@
         <v>18000000</v>
       </c>
       <c r="O2" t="n">
-        <v>11000000</v>
+        <v>12000000</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -1507,7 +1619,7 @@
         <v>0.04</v>
       </c>
       <c r="U2" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
@@ -1525,26 +1637,58 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tổng</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>197</v>
       </c>
       <c r="C3" t="n">
-        <v>1500000</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+        <v>1000000</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>08-24-2024</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>HD-LUXURY-538</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nâng mũi</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ngô Xuân Nhi</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Lâm Hoàng Phú</t>
+        </is>
+      </c>
       <c r="K3" t="n">
         <v>10000000</v>
       </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Đỗ Thị Huyền Trân</t>
+        </is>
+      </c>
       <c r="M3" t="n">
         <v>8000000</v>
       </c>
@@ -1552,10 +1696,16 @@
         <v>18000000</v>
       </c>
       <c r="O3" t="n">
-        <v>11000000</v>
-      </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
+        <v>12000000</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Lâm Thị Mỹ Hằng</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v/>
+      </c>
       <c r="R3" t="n">
         <v>0</v>
       </c>
@@ -1563,10 +1713,10 @@
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="U3" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
@@ -1578,6 +1728,65 @@
         <v>0</v>
       </c>
       <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tổng</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2500000</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="n">
+        <v>20000000</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>16000000</v>
+      </c>
+      <c r="N4" t="n">
+        <v>36000000</v>
+      </c>
+      <c r="O4" t="n">
+        <v>24000000</v>
+      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1647,7 +1856,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2622000</v>
+        <v>2992000</v>
       </c>
     </row>
     <row r="6">
@@ -1707,7 +1916,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1947,7 +2156,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>7550214.285714285</v>
+        <v>7880214.285714285</v>
       </c>
     </row>
     <row r="36">
@@ -1977,7 +2186,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>7550214.285714285</v>
+        <v>7880214.285714285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix big lương phụ phẫu 2 đơn thu nợ 1 tháng. Chưa fix được
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1003,35 +1003,147 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>683</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>08-25-2024</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Nguyễn Đặng Thảo Nhi</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Tiêm Filler</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>2800000</v>
+      </c>
+      <c r="I11" t="n">
+        <v/>
+      </c>
+      <c r="J11" t="n">
+        <v/>
+      </c>
+      <c r="K11" t="n">
+        <v>2800000</v>
+      </c>
+      <c r="L11" t="n">
+        <v>2800000</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>685</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>08-25-2024</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Nguyễn Thị Thoa</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Khách cũ</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Tiêm Filler</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="I12" t="n">
+        <v/>
+      </c>
+      <c r="J12" t="n">
+        <v/>
+      </c>
+      <c r="K12" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N12" t="n">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>9</v>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="n">
-        <v>28300000</v>
-      </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>28300000</v>
-      </c>
-      <c r="L11" t="n">
-        <v>29800000</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>2992000</v>
+      <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>32900000</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>32900000</v>
+      </c>
+      <c r="L13" t="n">
+        <v>34400000</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>3452000</v>
       </c>
     </row>
   </sheetData>
@@ -1045,7 +1157,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1360,35 +1472,93 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>686</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>08-25-2024</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Chị Sa</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Khách cũ</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Tiêm Filler</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Đỗ Thị Huyền Trân</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="L6" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N6" t="n">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="n">
         <v>1000000</v>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="n">
-        <v>13500000</v>
-      </c>
-      <c r="K6" t="n">
-        <v>14500000</v>
-      </c>
-      <c r="L6" t="n">
-        <v>14500000</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>510000</v>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>17500000</v>
+      </c>
+      <c r="K7" t="n">
+        <v>18500000</v>
+      </c>
+      <c r="L7" t="n">
+        <v>18500000</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>670000</v>
       </c>
     </row>
   </sheetData>
@@ -1619,7 +1789,7 @@
         <v>0.04</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
@@ -1716,7 +1886,7 @@
         <v>0.04</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
@@ -1775,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="V4" t="n">
         <v>0</v>
@@ -1826,7 +1996,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
@@ -1836,7 +2006,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>717500</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="4">
@@ -1846,7 +2016,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3660714.285714286</v>
+        <v>4285714.285714285</v>
       </c>
     </row>
     <row r="5">
@@ -1856,7 +2026,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2992000</v>
+        <v>3452000</v>
       </c>
     </row>
     <row r="6">
@@ -1866,7 +2036,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>510000</v>
+        <v>670000</v>
       </c>
     </row>
     <row r="7">
@@ -1916,7 +2086,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="12">
@@ -2156,7 +2326,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>7880214.285714285</v>
+        <v>9347714.285714285</v>
       </c>
     </row>
     <row r="36">
@@ -2186,7 +2356,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>7880214.285714285</v>
+        <v>9347714.285714285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixbug tinh chiết khấu đơn thu nợ
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
@@ -1789,7 +1789,7 @@
         <v>0.04</v>
       </c>
       <c r="U2" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
@@ -1945,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>100000</v>
+        <v>80000</v>
       </c>
       <c r="V4" t="n">
         <v>0</v>
@@ -2086,7 +2086,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>100000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="12">
@@ -2326,7 +2326,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>9347714.285714285</v>
+        <v>9327714.285714285</v>
       </c>
     </row>
     <row r="36">
@@ -2356,7 +2356,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>9347714.285714285</v>
+        <v>9327714.285714285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thêm chi tiết về ứng lương vào báo cảo tổng hợp
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v/>
+        <v>1500000</v>
       </c>
       <c r="I9" t="n">
         <v/>
@@ -932,7 +932,7 @@
         <v/>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>1500000</v>
       </c>
       <c r="L9" t="n">
         <v>1500000</v>
@@ -941,7 +941,7 @@
         <v>0.1</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="10">
@@ -1127,14 +1127,14 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
-        <v>32900000</v>
+        <v>34400000</v>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="n">
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>32900000</v>
+        <v>34400000</v>
       </c>
       <c r="L13" t="n">
         <v>34400000</v>
@@ -1143,7 +1143,7 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>3452000</v>
+        <v>3602000</v>
       </c>
     </row>
   </sheetData>
@@ -1157,7 +1157,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1530,35 +1530,93 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>695</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>08-27-2024</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Chị Sa</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Khách cũ</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Tiêm Filler</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Đỗ Thị Huyền Trân</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="K7" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="L7" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N7" t="n">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
         <v>1000000</v>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="n">
-        <v>17500000</v>
-      </c>
-      <c r="K7" t="n">
-        <v>18500000</v>
-      </c>
-      <c r="L7" t="n">
-        <v>18500000</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>670000</v>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>20500000</v>
+      </c>
+      <c r="K8" t="n">
+        <v>21500000</v>
+      </c>
+      <c r="L8" t="n">
+        <v>21500000</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>790000</v>
       </c>
     </row>
   </sheetData>
@@ -2026,7 +2084,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3452000</v>
+        <v>3602000</v>
       </c>
     </row>
     <row r="6">
@@ -2036,7 +2094,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>670000</v>
+        <v>790000</v>
       </c>
     </row>
     <row r="7">
@@ -2326,7 +2384,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>9327714.285714285</v>
+        <v>9597714.285714285</v>
       </c>
     </row>
     <row r="36">
@@ -2356,7 +2414,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>9327714.285714285</v>
+        <v>9597714.285714285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add thêm nhân sự Nguyễn Hữu Quang
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 8-2024.xlsx
@@ -2156,7 +2156,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -2166,7 +2166,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -2176,7 +2176,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5000000</v>
+        <v>5178571.428571429</v>
       </c>
     </row>
     <row r="4">
@@ -2486,7 +2486,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>10092000</v>
+        <v>10270571.42857143</v>
       </c>
     </row>
     <row r="35">
@@ -2516,7 +2516,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10092000</v>
+        <v>10270571.42857143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>